<commit_message>
Layout 75% complete for V0.1
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Teensy LC Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Teensy LC Pin Usage Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4071CB-4C3D-5542-A742-8C8D4F3E5A38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{AD4071CB-4C3D-5542-A742-8C8D4F3E5A38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{51EC6218-4C39-1746-8485-533B3DA56131}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19620" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
   <si>
     <t>Custom</t>
   </si>
@@ -225,9 +225,6 @@
     <t>3.3V Regulated VOUT from MCU</t>
   </si>
   <si>
-    <t>3.3V Regulated VOUT to AREF</t>
-  </si>
-  <si>
     <t xml:space="preserve">Battery Voltage (/2) monitor </t>
   </si>
   <si>
@@ -243,9 +240,6 @@
     <t>USB DATA ONLY VUSB JUMPER CUT</t>
   </si>
   <si>
-    <t>OLED Debug screen, hall sensors. Can this be shared with Transistor Matrix?</t>
-  </si>
-  <si>
     <t>Address 13 (shared with heartbeat)</t>
   </si>
   <si>
@@ -291,7 +285,25 @@
     <t>No Connection</t>
   </si>
   <si>
-    <t>Available</t>
+    <t>Hall Switch</t>
+  </si>
+  <si>
+    <t>OLED Debug screen, hall sensors.</t>
+  </si>
+  <si>
+    <t>3.3V Regulated VOUT to AREF and low power stuff</t>
+  </si>
+  <si>
+    <t>Pull high to avoid acceptable programming</t>
+  </si>
+  <si>
+    <t>VUSB</t>
+  </si>
+  <si>
+    <t>Power from USB to LiPo charger</t>
+  </si>
+  <si>
+    <t>LOGIC Ground</t>
   </si>
 </sst>
 </file>
@@ -1131,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B47D1C-78B7-5A42-A348-9E367CC3D141}">
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1162,7 +1174,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H2" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1225,12 +1237,12 @@
       </c>
       <c r="J4" s="7"/>
       <c r="P4" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="27" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>27</v>
@@ -1253,12 +1265,12 @@
       </c>
       <c r="J5" s="7"/>
       <c r="P5" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>27</v>
@@ -1281,12 +1293,12 @@
       </c>
       <c r="J6" s="7"/>
       <c r="P6" s="9" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F7" s="15">
         <v>2</v>
@@ -1319,7 +1331,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>27</v>
@@ -1358,7 +1370,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>27</v>
@@ -1391,7 +1403,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F10" s="15">
         <v>5</v>
@@ -1421,7 +1433,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>2</v>
@@ -1452,12 +1464,12 @@
         <v>27</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>18</v>
@@ -1485,12 +1497,12 @@
         <v>27</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>17</v>
@@ -1523,7 +1535,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>2</v>
@@ -1559,7 +1571,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>2</v>
@@ -1595,7 +1607,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>24</v>
@@ -1622,7 +1634,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>25</v>
@@ -1644,7 +1656,7 @@
         <v>62</v>
       </c>
       <c r="P17" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
@@ -1656,7 +1668,7 @@
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J18" s="7"/>
       <c r="P18" t="s">
@@ -1685,7 +1697,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>59</v>
@@ -1704,12 +1716,12 @@
         <v>43</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>59</v>
@@ -1733,7 +1745,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>59</v>
@@ -1742,15 +1754,17 @@
         <v>7</v>
       </c>
       <c r="H22" s="7"/>
-      <c r="I22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="J22" s="7"/>
       <c r="P22" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F23" s="15">
         <v>26</v>

</xml_diff>

<commit_message>
Digital and analog testing V0.1 PCB
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Teensy LC Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Teensy LC Pin Usage Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{AD4071CB-4C3D-5542-A742-8C8D4F3E5A38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{51EC6218-4C39-1746-8485-533B3DA56131}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{AD4071CB-4C3D-5542-A742-8C8D4F3E5A38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{09C6BEDC-6D3C-254F-B280-BF3DE2D3F35B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
@@ -1143,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B47D1C-78B7-5A42-A348-9E367CC3D141}">
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1397,7 +1397,7 @@
       <c r="M9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="P9" s="22" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1427,7 +1427,7 @@
       <c r="N10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="22" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       <c r="O13" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="P13" s="22" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added lots of documentation
BOM, Code plan, Dev plan, Electrical Block Diagram, Licensing analysis, Manufacturing considerations, schematic.
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Teensy LC Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Teensy LC Pin Usage Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{AD4071CB-4C3D-5542-A742-8C8D4F3E5A38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{09C6BEDC-6D3C-254F-B280-BF3DE2D3F35B}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{AD4071CB-4C3D-5542-A742-8C8D4F3E5A38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{B32BDBCB-2C85-0548-87D8-E58298B211E1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
@@ -177,30 +177,9 @@
     <t>SCK1</t>
   </si>
   <si>
-    <t>Address 14</t>
-  </si>
-  <si>
-    <t>Address 15</t>
-  </si>
-  <si>
-    <t>Address 16</t>
-  </si>
-  <si>
-    <t>Address 20</t>
-  </si>
-  <si>
-    <t>Address 19</t>
-  </si>
-  <si>
-    <t>Address 18</t>
-  </si>
-  <si>
     <t>LED Array (shared with address)</t>
   </si>
   <si>
-    <t>Address 17 (shared with LED Array)</t>
-  </si>
-  <si>
     <t>Vin (3.7-5.5)</t>
   </si>
   <si>
@@ -240,48 +219,9 @@
     <t>USB DATA ONLY VUSB JUMPER CUT</t>
   </si>
   <si>
-    <t>Address 13 (shared with heartbeat)</t>
-  </si>
-  <si>
-    <t>Address 1 - Q1P</t>
-  </si>
-  <si>
-    <t>Address 2 - Q1N</t>
-  </si>
-  <si>
     <t>SENSE_PULSE</t>
   </si>
   <si>
-    <t>Address 3 - Q2P</t>
-  </si>
-  <si>
-    <t>Address 4 - Q2N</t>
-  </si>
-  <si>
-    <t>Address 5 - Q3P</t>
-  </si>
-  <si>
-    <t>Address 6 - Q3N</t>
-  </si>
-  <si>
-    <t>Address 7 - Q4P</t>
-  </si>
-  <si>
-    <t>Address 8 - Q4N</t>
-  </si>
-  <si>
-    <t>Address 9 - Q5P</t>
-  </si>
-  <si>
-    <t>Address 10 - Q5N</t>
-  </si>
-  <si>
-    <t>Address 11 - Q6P</t>
-  </si>
-  <si>
-    <t>Address 12 - Q6N</t>
-  </si>
-  <si>
     <t>No Connection</t>
   </si>
   <si>
@@ -304,6 +244,66 @@
   </si>
   <si>
     <t>LOGIC Ground</t>
+  </si>
+  <si>
+    <t>Matrix Drive 1 - Q1P</t>
+  </si>
+  <si>
+    <t>Matrix Drive 2 - Q1N</t>
+  </si>
+  <si>
+    <t>Matrix Drive 3 - Q2P</t>
+  </si>
+  <si>
+    <t>Matrix Drive 4 - Q2N</t>
+  </si>
+  <si>
+    <t>Matrix Drive 5 - Q3P</t>
+  </si>
+  <si>
+    <t>Matrix Drive 6 - Q3N</t>
+  </si>
+  <si>
+    <t>Matrix Drive 7 - Q4P</t>
+  </si>
+  <si>
+    <t>Matrix Drive 8 - Q4N</t>
+  </si>
+  <si>
+    <t>Matrix Drive 9 - Q5P</t>
+  </si>
+  <si>
+    <t>Matrix Drive 10 - Q5N</t>
+  </si>
+  <si>
+    <t>Matrix Drive 11 - Q6P</t>
+  </si>
+  <si>
+    <t>Matrix Drive 12 - Q6N</t>
+  </si>
+  <si>
+    <t>Matrix Drive 13 Q7P (shared with heartbeat)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 15 Q8P</t>
+  </si>
+  <si>
+    <t>Matrix Drive 17 Q9P (shared with LED Array)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 19 Q10P</t>
+  </si>
+  <si>
+    <t>Matrix Drive 14 Q7N</t>
+  </si>
+  <si>
+    <t>Matrix Drive 16 Q8N</t>
+  </si>
+  <si>
+    <t>Matrix Drive 18 Q9N</t>
+  </si>
+  <si>
+    <t>Matrix Drive 20 Q10N</t>
   </si>
 </sst>
 </file>
@@ -1143,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B47D1C-78B7-5A42-A348-9E367CC3D141}">
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1174,7 +1174,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H2" s="21" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1226,23 +1226,23 @@
     </row>
     <row r="4" spans="1:16" ht="25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="J4" s="7"/>
       <c r="P4" s="20" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="27" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>27</v>
@@ -1265,12 +1265,12 @@
       </c>
       <c r="J5" s="7"/>
       <c r="P5" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>27</v>
@@ -1289,16 +1289,16 @@
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="J6" s="7"/>
       <c r="P6" s="9" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F7" s="15">
         <v>2</v>
@@ -1326,7 +1326,7 @@
         <v>27</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -1365,7 +1365,7 @@
         <v>27</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -1398,7 +1398,7 @@
         <v>20</v>
       </c>
       <c r="P9" s="22" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -1428,7 +1428,7 @@
         <v>2</v>
       </c>
       <c r="P10" s="22" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -1464,7 +1464,7 @@
         <v>27</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -1497,7 +1497,7 @@
         <v>27</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -1530,7 +1530,7 @@
         <v>27</v>
       </c>
       <c r="P13" s="22" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -1566,7 +1566,7 @@
         <v>27</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1602,7 +1602,7 @@
         <v>27</v>
       </c>
       <c r="P15" s="16" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -1629,7 +1629,7 @@
         <v>37</v>
       </c>
       <c r="P16" s="16" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -1653,31 +1653,31 @@
         <v>13</v>
       </c>
       <c r="M17" s="15" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="P17" s="16" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="18" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="J18" s="7"/>
       <c r="P18" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F19" s="15">
         <v>17</v>
@@ -1689,18 +1689,18 @@
         <v>11</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>6</v>
@@ -1716,15 +1716,15 @@
         <v>43</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>4</v>
@@ -1740,31 +1740,31 @@
         <v>44</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="4" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="J22" s="7"/>
       <c r="P22" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="F23" s="15">
         <v>26</v>
@@ -1776,7 +1776,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="7"/>
       <c r="P23" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added tab for Teensy 3.2 pin usage in v0.3 hardware.
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Teensy LC Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Teensy LC Pin Usage Mapping.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{AD4071CB-4C3D-5542-A742-8C8D4F3E5A38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{B32BDBCB-2C85-0548-87D8-E58298B211E1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6F7748-6035-094B-B1AC-3B83BC5A1626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="-51200" yWindow="-10340" windowWidth="51200" windowHeight="28340" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="v0.1-0.2 Teensy LC" sheetId="1" r:id="rId1"/>
+    <sheet name="v0.3 Teensy 3.2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="129">
   <si>
     <t>Custom</t>
   </si>
@@ -60,9 +63,6 @@
     <t>26/A12/DAC</t>
   </si>
   <si>
-    <t>Teensy LC Pinout Assignments</t>
-  </si>
-  <si>
     <t>SHORT EDGE</t>
   </si>
   <si>
@@ -304,13 +304,130 @@
   </si>
   <si>
     <t>Matrix Drive 20 Q10N</t>
+  </si>
+  <si>
+    <t>Teensy-LC delivers an impressive collection of capabilities to make modern electronic projects simpler. It features an ARM Cortex-M0+ processor at 48 MHz, 62K Flash, 8K RAM, 12 bit analog input &amp; output, hardware Serial, SPI &amp; I2C, USB, and a total of 27 I/O pins.</t>
+  </si>
+  <si>
+    <t>Upgrade path is Teensy 3.1 or 3.2</t>
+  </si>
+  <si>
+    <t>Version 3.2 features a 32 bit ARM processor.</t>
+  </si>
+  <si>
+    <t>Teensy 3.2 adds a more powerful 3.3 volt regulator, with the ability to directly power ESP8266 Wifi, WIZ820io Ethernet and other power-hungry 3.3V add-on boards.</t>
+  </si>
+  <si>
+    <t>The RAM has quadrupled since 3.0, from 16K to 64K.</t>
+  </si>
+  <si>
+    <t>Flash memory has also doubled, to 256K</t>
+  </si>
+  <si>
+    <t>All digital pins are 5 volt tolerant on Teensy 3.2 &amp; 3.1. However, the analog-only pins (A10-A14), AREF, Program and Reset are 3.3V only.</t>
+  </si>
+  <si>
+    <t>https://www.pjrc.com/teensy/teensy31.html</t>
+  </si>
+  <si>
+    <t>https://www.pjrc.com/teensy/teensyLC.html</t>
+  </si>
+  <si>
+    <t>Teensy LC Pinout Assignments for v0.1 and v0.2 Core 64 Badge</t>
+  </si>
+  <si>
+    <t>Teensy 3.2 Pinout Assignments for v0.3 Core 64 Badge</t>
+  </si>
+  <si>
+    <t>Core array matrix transistors 20+1=21 including Enable</t>
+  </si>
+  <si>
+    <t>3X using 3-to-8 decoder yields 24 outputs from 9 pins.</t>
+  </si>
+  <si>
+    <t>#22 and #23 could be used for a future active stylus</t>
+  </si>
+  <si>
+    <t>#24 available</t>
+  </si>
+  <si>
+    <t>Expand hall and reed to be 8 hall sensors.</t>
+  </si>
+  <si>
+    <t>LED Array</t>
+  </si>
+  <si>
+    <t>OLED (i2C)</t>
+  </si>
+  <si>
+    <t>v0.3 and beyond planning</t>
+  </si>
+  <si>
+    <t>TOTAL PINS NEED</t>
+  </si>
+  <si>
+    <t>Analog battery voltage</t>
+  </si>
+  <si>
+    <t>Int. capable, Sense (maybe 2 sense for CW and CCW discrimination?)</t>
+  </si>
+  <si>
+    <t>Heartbeat built-in LED</t>
+  </si>
+  <si>
+    <t>(or use CD4021B  https://www.arduino.cc/en/tutorial/ShiftIn)</t>
+  </si>
+  <si>
+    <t>SAO #1 (i2C, GND, 3.3V, and 2 GPIOS each)</t>
+  </si>
+  <si>
+    <t>(Or use CD4021B  https://www.arduino.cc/en/tutorial/ShiftIn)</t>
+  </si>
+  <si>
+    <t>(Or use 2x 16 GPIO I2C expander http://ww1.microchip.com/downloads/en/DeviceDoc/20090C.pdf)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 1 - Q1P (XB0-3)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 2 - Q1N (XB0-3)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 3 - Q2P (XB4-7)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 4 - Q2N (XB4-7)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 5 - Q3P (XT0,4)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 9 - Q5P (XT2,6)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 10 - Q5N (XT2,6)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 8 - Q4N (XT1,5)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 7 - Q4P (XT1,5)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 6 - Q3N (XT0,4)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 11 - Q6P (XT3,7)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 12 - Q6N (XT3,7)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -368,8 +485,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +524,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,10 +623,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -537,18 +677,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,16 +720,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>32821</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>157685</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1203035</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>94188</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1552595</xdr:colOff>
+      <xdr:colOff>1578429</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>15879</xdr:rowOff>
+      <xdr:rowOff>9077</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -607,8 +759,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="5400000">
-          <a:off x="5598330" y="1521614"/>
-          <a:ext cx="2993506" cy="1519774"/>
+          <a:off x="5619751" y="1165686"/>
+          <a:ext cx="2926603" cy="1581894"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -699,7 +851,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>55563</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>5602</xdr:rowOff>
+      <xdr:rowOff>5603</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -837,6 +989,364 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 5" descr="Image result for teensy lc backside">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A6EE199-8F91-D644-8506-F7CAEB1EBA6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6299200" y="3924300"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66222</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>117928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1569357</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9074</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8D62843-1F3D-A446-86F6-3A570BE3673C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="5400000">
+          <a:off x="5661931" y="1216933"/>
+          <a:ext cx="2902860" cy="1503135"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>54430</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>172357</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47210</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{725F2268-9C4C-354E-B6CE-41DE42F581BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6350001" y="5061857"/>
+          <a:ext cx="2795852" cy="1306286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>235858</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>84365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>943428</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>169637</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C41C1AE-FB4D-514C-B0E0-3869D4B102A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="5400000">
+          <a:off x="696686" y="4249966"/>
+          <a:ext cx="4874986" cy="5796641"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>907143</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>117928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>99786</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>166939</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5779CE2B-EB33-DC42-84AB-69BC07B6C2D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5996214" y="6141357"/>
+          <a:ext cx="3202215" cy="2643439"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>99785</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>72571</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47267</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3C87351-5E34-0747-B93E-26AEF1F70F3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9198428" y="4816929"/>
+          <a:ext cx="6422572" cy="6043481"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1141,10 +1651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B47D1C-78B7-5A42-A348-9E367CC3D141}">
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,12 +1679,15 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H2" s="21" t="s">
-        <v>61</v>
+      <c r="A2" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1191,10 +1704,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
@@ -1203,13 +1716,13 @@
         <v>5</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M3" s="15" t="s">
         <v>3</v>
@@ -1224,34 +1737,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4" s="7"/>
-      <c r="P4" s="20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="27" x14ac:dyDescent="0.2">
+      <c r="P4" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="15">
         <v>0</v>
@@ -1264,22 +1777,22 @@
         <v>4</v>
       </c>
       <c r="J5" s="7"/>
-      <c r="P5" s="19" t="s">
-        <v>59</v>
+      <c r="P5" s="22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="15">
         <v>1</v>
@@ -1289,16 +1802,16 @@
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J6" s="7"/>
       <c r="P6" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="15">
         <v>2</v>
@@ -1314,27 +1827,27 @@
         <v>23</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N7" s="15" t="s">
         <v>2</v>
       </c>
       <c r="O7" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="22" t="s">
-        <v>54</v>
+        <v>26</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>2</v>
@@ -1353,27 +1866,27 @@
         <v>22</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N8" s="15" t="s">
         <v>2</v>
       </c>
       <c r="O8" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>2</v>
@@ -1392,18 +1905,18 @@
         <v>21</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="P9" s="22" t="s">
-        <v>86</v>
+        <v>19</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F10" s="15">
         <v>5</v>
@@ -1419,27 +1932,27 @@
         <v>20</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="22" t="s">
-        <v>89</v>
+      <c r="P10" s="20" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" s="15">
         <v>6</v>
@@ -1455,24 +1968,24 @@
         <v>19</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O11" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F12" s="15">
         <v>7</v>
@@ -1488,24 +2001,24 @@
         <v>18</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O12" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="15">
         <v>8</v>
@@ -1521,27 +2034,27 @@
         <v>17</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N13" s="15" t="s">
         <v>2</v>
       </c>
       <c r="O13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="22" t="s">
-        <v>85</v>
+        <v>26</v>
+      </c>
+      <c r="P13" s="20" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" s="15">
         <v>9</v>
@@ -1557,30 +2070,30 @@
         <v>16</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N14" s="15" t="s">
         <v>2</v>
       </c>
       <c r="O14" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="15">
         <v>10</v>
@@ -1596,21 +2109,21 @@
         <v>15</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O15" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P15" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="15">
         <v>11</v>
@@ -1626,18 +2139,18 @@
         <v>14</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P16" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="15">
         <v>12</v>
@@ -1647,60 +2160,60 @@
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J17" s="7">
         <v>13</v>
       </c>
       <c r="M17" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P17" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J18" s="7"/>
       <c r="P18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="15">
         <v>17</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>6</v>
@@ -1713,18 +2226,18 @@
         <v>24</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>4</v>
@@ -1737,34 +2250,34 @@
         <v>25</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J22" s="7"/>
       <c r="P22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F23" s="15">
         <v>26</v>
@@ -1776,7 +2289,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="7"/>
       <c r="P23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
@@ -1893,9 +2406,1068 @@
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
     </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E716DB14-6730-2649-97D0-3B89A33A4A44}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
+  <dimension ref="A1:Z53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="U27" sqref="U27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="15"/>
+    <col min="3" max="3" width="5.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="15"/>
+    <col min="16" max="16" width="29.5" customWidth="1"/>
+    <col min="19" max="20" width="10.83203125" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="P4" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="26"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="P5" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="15">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="P6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="15">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="4">
+        <v>23</v>
+      </c>
+      <c r="J7" s="7">
+        <v>23</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="25">
+        <v>9</v>
+      </c>
+      <c r="T7" s="25"/>
+      <c r="U7" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="V7" s="26"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="15">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="4">
+        <v>22</v>
+      </c>
+      <c r="J8" s="7">
+        <v>22</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="V8" s="26"/>
+      <c r="W8" s="26"/>
+      <c r="X8" s="26"/>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="26"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="15">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="4">
+        <v>21</v>
+      </c>
+      <c r="J9" s="7">
+        <v>21</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="26"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="15">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3">
+        <v>5</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="4">
+        <v>20</v>
+      </c>
+      <c r="J10" s="7">
+        <v>20</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="V10" s="26"/>
+      <c r="W10" s="26"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="26"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="15">
+        <v>6</v>
+      </c>
+      <c r="G11" s="3">
+        <v>6</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="4">
+        <v>19</v>
+      </c>
+      <c r="J11" s="7">
+        <v>19</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="S11" s="25">
+        <v>2</v>
+      </c>
+      <c r="T11" s="25">
+        <v>2</v>
+      </c>
+      <c r="U11" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="15">
+        <v>7</v>
+      </c>
+      <c r="G12" s="3">
+        <v>7</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="4">
+        <v>18</v>
+      </c>
+      <c r="J12" s="7">
+        <v>18</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="15">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3">
+        <v>8</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="4">
+        <v>17</v>
+      </c>
+      <c r="J13" s="7">
+        <v>17</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="S13" s="25">
+        <v>8</v>
+      </c>
+      <c r="T13" s="25"/>
+      <c r="U13" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="15">
+        <v>9</v>
+      </c>
+      <c r="G14" s="3">
+        <v>9</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="4">
+        <v>16</v>
+      </c>
+      <c r="J14" s="7">
+        <v>16</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P14" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="15">
+        <v>10</v>
+      </c>
+      <c r="G15" s="3">
+        <v>10</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="4">
+        <v>15</v>
+      </c>
+      <c r="J15" s="7">
+        <v>15</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P15" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="26"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="15">
+        <v>11</v>
+      </c>
+      <c r="G16" s="3">
+        <v>11</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="4">
+        <v>14</v>
+      </c>
+      <c r="J16" s="7">
+        <v>14</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="P16" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="S16" s="25">
+        <v>2</v>
+      </c>
+      <c r="T16" s="25">
+        <v>2</v>
+      </c>
+      <c r="U16" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="V16" s="26"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="26"/>
+      <c r="Y16" s="26"/>
+      <c r="Z16" s="26"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="15">
+        <v>12</v>
+      </c>
+      <c r="G17" s="3">
+        <v>12</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="7">
+        <v>13</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="P17" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="S17" s="25">
+        <v>2</v>
+      </c>
+      <c r="T17" s="25">
+        <v>2</v>
+      </c>
+      <c r="U17" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="26"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="7"/>
+      <c r="P18" t="s">
+        <v>51</v>
+      </c>
+      <c r="S18" s="25">
+        <v>1</v>
+      </c>
+      <c r="T18" s="25">
+        <v>1</v>
+      </c>
+      <c r="U18" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="V18" s="26"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="26"/>
+      <c r="Y18" s="26"/>
+      <c r="Z18" s="26"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="15">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="S19" s="25">
+        <v>1</v>
+      </c>
+      <c r="T19" s="25">
+        <v>1</v>
+      </c>
+      <c r="U19" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="26"/>
+      <c r="Z19" s="26"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="4">
+        <v>24</v>
+      </c>
+      <c r="J20" s="7">
+        <v>24</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="S20" s="25">
+        <v>1</v>
+      </c>
+      <c r="T20" s="25">
+        <v>1</v>
+      </c>
+      <c r="U20" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="26"/>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="26"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="4">
+        <v>25</v>
+      </c>
+      <c r="J21" s="7">
+        <v>25</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="P21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="S21" s="25"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="26"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="26"/>
+      <c r="Y21" s="26"/>
+      <c r="Z21" s="26"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" s="7"/>
+      <c r="P22" t="s">
+        <v>68</v>
+      </c>
+      <c r="S22" s="25"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
+      <c r="Y22" s="26"/>
+      <c r="Z22" s="26"/>
+    </row>
+    <row r="23" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="15">
+        <v>26</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="14"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="7"/>
+      <c r="P23" t="s">
+        <v>51</v>
+      </c>
+      <c r="S23" s="25">
+        <f>SUM(S7:S22)</f>
+        <v>26</v>
+      </c>
+      <c r="T23" s="29">
+        <f>SUM(T7:T22)</f>
+        <v>9</v>
+      </c>
+      <c r="U23" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="26"/>
+      <c r="Z23" s="26"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
+      <c r="Y24" s="26"/>
+      <c r="Z24" s="26"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="H25" s="10"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="26"/>
+      <c r="V25" s="26"/>
+      <c r="W25" s="26"/>
+      <c r="X25" s="26"/>
+      <c r="Y25" s="26"/>
+      <c r="Z25" s="26"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="S26" s="25"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="11"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="S4:Y4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CF74EE04-8972-D048-A403-865EBF5C5826}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Feather to Teensy Adapter data, working on new pin mapping
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Teensy LC Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Teensy LC Pin Usage Mapping.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6F7748-6035-094B-B1AC-3B83BC5A1626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE26E159-2833-A84D-AA39-0FFABBC06F23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-10340" windowWidth="51200" windowHeight="28340" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="-51220" yWindow="-10340" windowWidth="51200" windowHeight="28340" activeTab="2" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="v0.1-0.2 Teensy LC" sheetId="1" r:id="rId1"/>
-    <sheet name="v0.3 Teensy 3.2" sheetId="2" r:id="rId2"/>
+    <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
+    <sheet name="v0.1-0.2 Teensy LC" sheetId="1" r:id="rId2"/>
+    <sheet name="v0.3 Teensy LC and 3.2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="132">
   <si>
     <t>Custom</t>
   </si>
@@ -421,6 +422,15 @@
   </si>
   <si>
     <t>Matrix Drive 12 - Q6N (XT3,7)</t>
+  </si>
+  <si>
+    <t>https://forum.pjrc.com/threads/55568-Teensy-3-2-3-5-pin-compatibility</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/u/0/d/1LSi0c17iqtvpKuNSYksMG306_FpWdJcniSRR6aGNNYQ/htmlview#</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1LSi0c17iqtvpKuNSYksMG306_FpWdJcniSRR6aGNNYQ/edit#gid=1683806103</t>
   </si>
 </sst>
 </file>
@@ -691,11 +701,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1650,6 +1660,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB4F958-3252-A747-BA09-0BFF739A014F}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{968E6DDA-28C4-FC49-8683-06B8524D89AD}"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://docs.google.com/spreadsheets/u/0/d/1LSi0c17iqtvpKuNSYksMG306_FpWdJcniSRR6aGNNYQ/htmlview" xr:uid="{8CAE2451-52BB-394E-8469-BD7C21D84CB9}"/>
+    <hyperlink ref="A3" r:id="rId3" location="gid=1683806103" display="https://docs.google.com/spreadsheets/d/1LSi0c17iqtvpKuNSYksMG306_FpWdJcniSRR6aGNNYQ/edit - gid=1683806103" xr:uid="{FE7FFB1A-8400-9D45-BC4B-B4A5C3A5292E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B47D1C-78B7-5A42-A348-9E367CC3D141}">
   <dimension ref="A1:P50"/>
   <sheetViews>
@@ -2426,7 +2471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:Z53"/>
   <sheetViews>
@@ -2531,15 +2576,15 @@
       <c r="P4" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S4" s="27" t="s">
+      <c r="S4" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="29"/>
+      <c r="Y4" s="29"/>
       <c r="Z4" s="26"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -3012,7 +3057,7 @@
       </c>
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
-      <c r="U15" s="28" t="s">
+      <c r="U15" s="27" t="s">
         <v>116</v>
       </c>
       <c r="V15" s="26"/>
@@ -3284,7 +3329,7 @@
         <f>SUM(S7:S22)</f>
         <v>26</v>
       </c>
-      <c r="T23" s="29">
+      <c r="T23" s="28">
         <f>SUM(T7:T22)</f>
         <v>9</v>
       </c>

</xml_diff>